<commit_message>
Gráfico de Bolsa de Valores
</commit_message>
<xml_diff>
--- a/7-Gráficos/26. Gráfico de Bolsa de Valores - Material(1).xlsx
+++ b/7-Gráficos/26. Gráfico de Bolsa de Valores - Material(1).xlsx
@@ -1,34 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaof\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\cursos\excel\7-Gráficos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D623CF6-F25B-4AE6-B3A8-24FC04C680F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7CEBDE-46AC-481A-8F1C-36C8C37902D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{25E5CC15-4B2E-4140-8F38-E3ADA3265091}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{25E5CC15-4B2E-4140-8F38-E3ADA3265091}"/>
   </bookViews>
   <sheets>
     <sheet name="Gabarito" sheetId="2" r:id="rId1"/>
     <sheet name="DoZero" sheetId="3" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">DoZero!$A$2:$A$56</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">DoZero!$B$1</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">DoZero!$F$2:$F$56</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">DoZero!$B$2:$B$56</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">DoZero!$C$1</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">DoZero!$C$2:$C$56</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">DoZero!$D$1</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">DoZero!$D$2:$D$56</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">DoZero!$E$1</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">DoZero!$E$2:$E$56</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">DoZero!$F$1</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -42,6 +29,9 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -170,7 +160,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -204,9 +194,6 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -216,14 +203,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF8181"/>
+          <bgColor rgb="FF47FF9A"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF47FF9A"/>
+          <bgColor rgb="FFFF8181"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2548,777 +2535,9 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:areaChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>DoZero!$E$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Aux3</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="4BFF9C"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:cat>
-            <c:numRef>
-              <c:f>DoZero!$A$2:$A$56</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="55"/>
-                <c:pt idx="0">
-                  <c:v>44200</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>44201</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>44202</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>44203</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>44204</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>44207</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>44208</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>44209</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>44210</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>44211</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>44214</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>44215</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>44216</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>44217</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>44218</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>44222</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>44223</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>44224</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>44225</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>44228</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>44229</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>44230</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>44231</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>44232</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>44235</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>44236</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>44237</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>44238</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>44239</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>44244</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>44245</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>44246</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>44249</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>44250</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>44251</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>44252</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>44253</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>44256</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>44257</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>44258</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>44259</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>44260</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>44263</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>44264</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>44265</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>44266</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>44267</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>44270</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>44271</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>44272</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>44273</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>44274</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>44277</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>44278</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>44279</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>DoZero!$E$2:$E$56</c:f>
-              <c:numCache>
-                <c:formatCode>"R$"\ #,##0.00</c:formatCode>
-                <c:ptCount val="55"/>
-                <c:pt idx="0">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-FE89-4D99-B6AA-B7E08DAA2922}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>DoZero!$F$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Aux4</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="FF5B5B"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:cat>
-            <c:numRef>
-              <c:f>DoZero!$A$2:$A$56</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="55"/>
-                <c:pt idx="0">
-                  <c:v>44200</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>44201</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>44202</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>44203</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>44204</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>44207</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>44208</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>44209</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>44210</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>44211</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>44214</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>44215</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>44216</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>44217</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>44218</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>44222</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>44223</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>44224</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>44225</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>44228</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>44229</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>44230</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>44231</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>44232</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>44235</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>44236</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>44237</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>44238</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>44239</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>44244</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>44245</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>44246</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>44249</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>44250</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>44251</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>44252</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>44253</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>44256</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>44257</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>44258</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>44259</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>44260</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>44263</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>44264</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>44265</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>44266</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>44267</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>44270</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>44271</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>44272</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>44273</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>44274</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>44277</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>44278</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>44279</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>DoZero!$F$2:$F$56</c:f>
-              <c:numCache>
-                <c:formatCode>"R$"\ #,##0.00</c:formatCode>
-                <c:ptCount val="55"/>
-                <c:pt idx="0">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>113.06</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>113.85</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>115.25</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>114.62</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>115.82</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>115.18</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>114.91</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>113.92</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>114.9</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>115.05</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>115.86</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>114.61</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>113.82</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>108.25</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>110.76</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>111.46</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-FE89-4D99-B6AA-B7E08DAA2922}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="156679088"/>
-        <c:axId val="156680336"/>
-      </c:areaChart>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -3337,12 +2556,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="9525" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -3702,7 +2918,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-FE89-4D99-B6AA-B7E08DAA2922}"/>
+              <c16:uniqueId val="{00000000-3009-4D3D-93C2-79A700B4EB0F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3722,7 +2938,9 @@
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -3731,14 +2949,11 @@
             <c:symbol val="circle"/>
             <c:size val="12"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="bg1">
-                  <a:lumMod val="75000"/>
-                  <a:alpha val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
+              <a:noFill/>
               <a:ln w="9525">
-                <a:noFill/>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -3924,169 +3139,169 @@
                 <c:formatCode>"R$"\ #,##0.00</c:formatCode>
                 <c:ptCount val="55"/>
                 <c:pt idx="0">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>113.06</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>#N/A</c:v>
+                  <c:v>105.94</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4094,7 +3309,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-FE89-4D99-B6AA-B7E08DAA2922}"/>
+              <c16:uniqueId val="{00000001-3009-4D3D-93C2-79A700B4EB0F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4114,26 +3329,15 @@
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="12"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="bg1">
-                  <a:lumMod val="75000"/>
-                  <a:alpha val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -4316,169 +3520,169 @@
                 <c:formatCode>"R$"\ #,##0.00</c:formatCode>
                 <c:ptCount val="55"/>
                 <c:pt idx="0">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>#N/A</c:v>
+                  <c:v>114.55</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>111.46</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4486,7 +3690,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-FE89-4D99-B6AA-B7E08DAA2922}"/>
+              <c16:uniqueId val="{00000002-3009-4D3D-93C2-79A700B4EB0F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4498,13 +3702,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="156679088"/>
-        <c:axId val="156680336"/>
+        <c:axId val="1460089935"/>
+        <c:axId val="1460095215"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="156679088"/>
+        <c:axId val="1460089935"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4547,14 +3750,14 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="156680336"/>
+        <c:crossAx val="1460095215"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="156680336"/>
+        <c:axId val="1460095215"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4564,8 +3767,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="bg1">
-                  <a:lumMod val="95000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -4604,7 +3808,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="156679088"/>
+        <c:crossAx val="1460089935"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4616,7 +3820,7 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:plotVisOnly val="0"/>
+    <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
@@ -6149,27 +5353,29 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>579120</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>37768</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>293866</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1">
+        <xdr:cNvPr id="3" name="Gráfico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2604F025-8852-4D5C-A892-79C6E9EDC01E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29DA77EA-DA41-49DA-8ADA-9681BBE23DE1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -6190,19 +5396,19 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.84415</cdr:x>
-      <cdr:y>0.0525</cdr:y>
+      <cdr:x>0.79565</cdr:x>
+      <cdr:y>0.01299</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.96774</cdr:x>
-      <cdr:y>0.15165</cdr:y>
+      <cdr:x>0.97609</cdr:x>
+      <cdr:y>0.17208</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="DoZero!$L$2">
       <cdr:nvSpPr>
         <cdr:cNvPr id="2" name="CaixaDeTexto 1">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A787B3E-9FE9-46B6-8CD6-DD91B6BE3A09}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD007280-1E02-1BE7-6E13-D480C6100816}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -6210,20 +5416,20 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="6957061" y="181223"/>
-          <a:ext cx="1018610" cy="342311"/>
+          <a:off x="6972300" y="38100"/>
+          <a:ext cx="1581150" cy="466725"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </cdr:spPr>
       <cdr:txBody>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0" anchor="ctr"/>
         <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:pPr algn="ctr"/>
-          <a:fld id="{3945AFBF-7386-42D3-B290-741997745183}" type="TxLink">
-            <a:rPr lang="en-US" sz="1800" b="1" i="0" u="none" strike="noStrike">
+          <a:fld id="{29467BB8-3B1C-47CC-A9DC-CE8DE9D83927}" type="TxLink">
+            <a:rPr lang="en-US" sz="2000" b="1" i="0" u="none" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -6231,9 +5437,9 @@
               <a:cs typeface="Calibri"/>
             </a:rPr>
             <a:pPr algn="ctr"/>
-            <a:t>-1,42%</a:t>
+            <a:t>8,13%</a:t>
           </a:fld>
-          <a:endParaRPr lang="pt-BR" sz="1800" b="1"/>
+          <a:endParaRPr lang="pt-BR" sz="2000" b="1"/>
         </a:p>
       </cdr:txBody>
     </cdr:sp>
@@ -6242,9 +5448,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -6282,7 +5488,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -6388,7 +5594,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6530,7 +5736,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -6540,23 +5746,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8D9FA79-08E5-4A11-89F3-621F62BC40AC}">
   <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A10" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="1" customWidth="1"/>
     <col min="3" max="6" width="12" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="13.88671875" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" customWidth="1"/>
     <col min="9" max="9" width="2" customWidth="1"/>
-    <col min="10" max="10" width="13.88671875" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" customWidth="1"/>
     <col min="11" max="11" width="2" customWidth="1"/>
-    <col min="12" max="12" width="13.88671875" customWidth="1"/>
-    <col min="15" max="15" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" customWidth="1"/>
+    <col min="15" max="15" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -6587,7 +5795,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>44200</v>
       </c>
@@ -6628,7 +5836,7 @@
       </c>
       <c r="O2" s="4"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>44201</v>
       </c>
@@ -6666,7 +5874,7 @@
         <v>8.3500000000000085</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>44202</v>
       </c>
@@ -6690,7 +5898,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>44203</v>
       </c>
@@ -6714,7 +5922,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>44204</v>
       </c>
@@ -6738,7 +5946,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>44207</v>
       </c>
@@ -6762,7 +5970,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>44208</v>
       </c>
@@ -6786,7 +5994,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>44209</v>
       </c>
@@ -6810,7 +6018,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>44210</v>
       </c>
@@ -6834,7 +6042,7 @@
         <v>118.68</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>44211</v>
       </c>
@@ -6858,7 +6066,7 @@
         <v>115.78</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>44214</v>
       </c>
@@ -6882,7 +6090,7 @@
         <v>116.54</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>44215</v>
       </c>
@@ -6906,7 +6114,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>44216</v>
       </c>
@@ -6930,7 +6138,7 @@
         <v>115.24</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>44217</v>
       </c>
@@ -6954,7 +6162,7 @@
         <v>113.81</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>44218</v>
       </c>
@@ -6978,7 +6186,7 @@
         <v>113.18</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>44222</v>
       </c>
@@ -7002,7 +6210,7 @@
         <v>112.08</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>44223</v>
       </c>
@@ -7026,7 +6234,7 @@
         <v>110.96</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>44224</v>
       </c>
@@ -7050,7 +6258,7 @@
         <v>114.51</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>44225</v>
       </c>
@@ -7074,7 +6282,7 @@
         <v>110.56</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>44228</v>
       </c>
@@ -7098,7 +6306,7 @@
         <v>113.06</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>44229</v>
       </c>
@@ -7122,7 +6330,7 @@
         <v>113.85</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>44230</v>
       </c>
@@ -7146,7 +6354,7 @@
         <v>115.25</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>44231</v>
       </c>
@@ -7170,7 +6378,7 @@
         <v>114.62</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>44232</v>
       </c>
@@ -7194,7 +6402,7 @@
         <v>115.82</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>44235</v>
       </c>
@@ -7218,7 +6426,7 @@
         <v>115.18</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>44236</v>
       </c>
@@ -7242,7 +6450,7 @@
         <v>114.91</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>44237</v>
       </c>
@@ -7266,7 +6474,7 @@
         <v>113.92</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>44238</v>
       </c>
@@ -7290,7 +6498,7 @@
         <v>114.9</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>44239</v>
       </c>
@@ -7314,7 +6522,7 @@
         <v>115.05</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>44244</v>
       </c>
@@ -7338,7 +6546,7 @@
         <v>115.86</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>44245</v>
       </c>
@@ -7362,7 +6570,7 @@
         <v>114.61</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>44246</v>
       </c>
@@ -7386,7 +6594,7 @@
         <v>113.82</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>44249</v>
       </c>
@@ -7410,7 +6618,7 @@
         <v>108.25</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>44250</v>
       </c>
@@ -7434,7 +6642,7 @@
         <v>110.76</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>44251</v>
       </c>
@@ -7458,7 +6666,7 @@
         <v>111.46</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>44252</v>
       </c>
@@ -7482,7 +6690,7 @@
         <v>107.53</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>44253</v>
       </c>
@@ -7506,7 +6714,7 @@
         <v>105.59</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>44256</v>
       </c>
@@ -7530,7 +6738,7 @@
         <v>105.94</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>44257</v>
       </c>
@@ -7554,7 +6762,7 @@
         <v>107.5</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>44258</v>
       </c>
@@ -7578,7 +6786,7 @@
         <v>107.16</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>44259</v>
       </c>
@@ -7602,7 +6810,7 @@
         <v>108.57</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>44260</v>
       </c>
@@ -7626,7 +6834,7 @@
         <v>110.93</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>44263</v>
       </c>
@@ -7650,7 +6858,7 @@
         <v>105.35</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44264</v>
       </c>
@@ -7674,7 +6882,7 @@
         <v>107.19</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>44265</v>
       </c>
@@ -7698,7 +6906,7 @@
         <v>108.63</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>44266</v>
       </c>
@@ -7722,7 +6930,7 @@
         <v>110.45</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>44267</v>
       </c>
@@ -7746,7 +6954,7 @@
         <v>109.68</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>44270</v>
       </c>
@@ -7770,7 +6978,7 @@
         <v>110.66</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>44271</v>
       </c>
@@ -7794,7 +7002,7 @@
         <v>109.69</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>44272</v>
       </c>
@@ -7818,7 +7026,7 @@
         <v>112.05</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>44273</v>
       </c>
@@ -7842,7 +7050,7 @@
         <v>110.5</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>44274</v>
       </c>
@@ -7866,7 +7074,7 @@
         <v>111.7</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>44277</v>
       </c>
@@ -7890,7 +7098,7 @@
         <v>110.69</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>44278</v>
       </c>
@@ -7914,7 +7122,7 @@
         <v>109.02</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>44279</v>
       </c>
@@ -7962,528 +7170,418 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6DC53B9-EBCE-429D-8CC4-4E1B53EBCAA8}">
   <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="1" customWidth="1"/>
-    <col min="3" max="6" width="10.5546875" customWidth="1"/>
-    <col min="8" max="8" width="13.21875" customWidth="1"/>
-    <col min="9" max="9" width="2.33203125" customWidth="1"/>
-    <col min="10" max="10" width="13.21875" customWidth="1"/>
-    <col min="11" max="11" width="2.33203125" customWidth="1"/>
-    <col min="12" max="12" width="13.21875" customWidth="1"/>
+    <col min="3" max="6" width="10.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="16.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="2.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="2.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>44200</v>
       </c>
       <c r="B2" s="3">
         <v>114.09</v>
       </c>
-      <c r="C2" s="3" t="e">
-        <f>IF($H$2=A2,B2,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D2" s="3" t="e">
-        <f>IF(A2=$J$2,B2,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E2" s="3" t="e">
-        <f>IF(AND(A2&gt;=$H$2,A2&lt;=$J$2,$L$2&gt;=0),B2,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F2" s="3" t="e">
-        <f>IF(AND(A2&gt;=$H$2,A2&lt;=$J$2,$L$2&lt;0),B2,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H2" s="13">
-        <v>44228</v>
-      </c>
-      <c r="J2" s="13">
-        <v>44251</v>
+      <c r="C2" s="3">
+        <f>IF($H$2=A2, B2, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
+        <f>IF($J$2 = A2, B2, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="H2" s="2">
+        <v>44256</v>
+      </c>
+      <c r="J2" s="2">
+        <v>44202</v>
       </c>
       <c r="L2" s="12">
-        <f>J3/H3-1</f>
-        <v>-1.4151777817088318E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+        <f>J3 / H3-1</f>
+        <v>8.1272418350009534E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>44201</v>
       </c>
       <c r="B3" s="3">
         <v>114.69</v>
       </c>
-      <c r="C3" s="3" t="e">
-        <f t="shared" ref="C3:C56" si="0">IF($H$2=A3,B3,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D3" s="3" t="e">
-        <f t="shared" ref="D3:D56" si="1">IF(A3=$J$2,B3,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E3" s="3" t="e">
-        <f t="shared" ref="E3:E56" si="2">IF(AND(A3&gt;=$H$2,A3&lt;=$J$2,$L$2&gt;=0),B3,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F3" s="3" t="e">
-        <f t="shared" ref="F3:F56" si="3">IF(AND(A3&gt;=$H$2,A3&lt;=$J$2,$L$2&lt;0),B3,#N/A)</f>
-        <v>#N/A</v>
-      </c>
+      <c r="C3" s="3">
+        <f t="shared" ref="C3:C56" si="0">IF($H$2=A3, B3, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
+        <f t="shared" ref="D3:D56" si="1">IF($J$2 = A3, B3, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
       <c r="H3" s="3">
-        <f>VLOOKUP(H2,A:B,2,0)</f>
-        <v>113.06</v>
-      </c>
-      <c r="J3" s="1">
-        <f>VLOOKUP(J2,A:B,2,0)</f>
-        <v>111.46</v>
+        <f>VLOOKUP(H2, A:B, 2, 0)</f>
+        <v>105.94</v>
+      </c>
+      <c r="J3" s="3">
+        <f>VLOOKUP(J2, A:B, 2, 0)</f>
+        <v>114.55</v>
       </c>
       <c r="L3" s="3">
-        <f>J3-H3</f>
-        <v>-1.6000000000000085</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+        <f>J3 - H3</f>
+        <v>8.61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>44202</v>
       </c>
       <c r="B4" s="3">
         <v>114.55</v>
       </c>
-      <c r="C4" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D4" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E4" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F4" s="3" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C4" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
+        <f t="shared" si="1"/>
+        <v>114.55</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>44203</v>
       </c>
       <c r="B5" s="3">
         <v>118.37</v>
       </c>
-      <c r="C5" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D5" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E5" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F5" s="3" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C5" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>44204</v>
       </c>
       <c r="B6" s="3">
         <v>120.4</v>
       </c>
-      <c r="C6" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D6" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E6" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F6" s="3" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C6" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>44207</v>
       </c>
       <c r="B7" s="3">
         <v>118.62</v>
       </c>
-      <c r="C7" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D7" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E7" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F7" s="3" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C7" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>44208</v>
       </c>
       <c r="B8" s="3">
         <v>119.45</v>
       </c>
-      <c r="C8" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D8" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E8" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F8" s="3" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C8" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>44209</v>
       </c>
       <c r="B9" s="3">
         <v>117.36</v>
       </c>
-      <c r="C9" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D9" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E9" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F9" s="3" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C9" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>44210</v>
       </c>
       <c r="B10" s="3">
         <v>118.68</v>
       </c>
-      <c r="C10" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D10" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E10" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F10" s="3" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C10" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>44211</v>
       </c>
       <c r="B11" s="3">
         <v>115.78</v>
       </c>
-      <c r="C11" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D11" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E11" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F11" s="3" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C11" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>44214</v>
       </c>
       <c r="B12" s="3">
         <v>116.54</v>
       </c>
-      <c r="C12" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D12" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E12" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F12" s="3" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C12" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>44215</v>
       </c>
       <c r="B13" s="3">
         <v>116</v>
       </c>
-      <c r="C13" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D13" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E13" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F13" s="3" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C13" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>44216</v>
       </c>
       <c r="B14" s="3">
         <v>115.24</v>
       </c>
-      <c r="C14" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D14" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E14" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F14" s="3" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C14" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>44217</v>
       </c>
       <c r="B15" s="3">
         <v>113.81</v>
       </c>
-      <c r="C15" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D15" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E15" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F15" s="3" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C15" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>44218</v>
       </c>
       <c r="B16" s="3">
         <v>113.18</v>
       </c>
-      <c r="C16" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D16" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E16" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F16" s="3" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C16" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>44222</v>
       </c>
       <c r="B17" s="3">
         <v>112.08</v>
       </c>
-      <c r="C17" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D17" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E17" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F17" s="3" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C17" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>44223</v>
       </c>
       <c r="B18" s="3">
         <v>110.96</v>
       </c>
-      <c r="C18" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D18" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E18" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F18" s="3" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C18" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>44224</v>
       </c>
       <c r="B19" s="3">
         <v>114.51</v>
       </c>
-      <c r="C19" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D19" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E19" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F19" s="3" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C19" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D19" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>44225</v>
       </c>
       <c r="B20" s="3">
         <v>110.56</v>
       </c>
-      <c r="C20" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D20" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E20" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F20" s="3" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C20" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D20" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>44228</v>
       </c>
@@ -8492,868 +7590,652 @@
       </c>
       <c r="C21" s="3">
         <f t="shared" si="0"/>
-        <v>113.06</v>
-      </c>
-      <c r="D21" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E21" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F21" s="3">
-        <f t="shared" si="3"/>
-        <v>113.06</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="D21" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>44229</v>
       </c>
       <c r="B22" s="3">
         <v>113.85</v>
       </c>
-      <c r="C22" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D22" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E22" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F22" s="3">
-        <f t="shared" si="3"/>
-        <v>113.85</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C22" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D22" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>44230</v>
       </c>
       <c r="B23" s="3">
         <v>115.25</v>
       </c>
-      <c r="C23" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D23" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E23" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F23" s="3">
-        <f t="shared" si="3"/>
-        <v>115.25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C23" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D23" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>44231</v>
       </c>
       <c r="B24" s="3">
         <v>114.62</v>
       </c>
-      <c r="C24" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D24" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E24" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F24" s="3">
-        <f t="shared" si="3"/>
-        <v>114.62</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C24" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D24" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>44232</v>
       </c>
       <c r="B25" s="3">
         <v>115.82</v>
       </c>
-      <c r="C25" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D25" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E25" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F25" s="3">
-        <f t="shared" si="3"/>
-        <v>115.82</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C25" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D25" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>44235</v>
       </c>
       <c r="B26" s="3">
         <v>115.18</v>
       </c>
-      <c r="C26" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D26" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E26" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F26" s="3">
-        <f t="shared" si="3"/>
-        <v>115.18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C26" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D26" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>44236</v>
       </c>
       <c r="B27" s="3">
         <v>114.91</v>
       </c>
-      <c r="C27" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D27" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E27" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F27" s="3">
-        <f t="shared" si="3"/>
-        <v>114.91</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C27" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D27" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>44237</v>
       </c>
       <c r="B28" s="3">
         <v>113.92</v>
       </c>
-      <c r="C28" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D28" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E28" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F28" s="3">
-        <f t="shared" si="3"/>
-        <v>113.92</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C28" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D28" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>44238</v>
       </c>
       <c r="B29" s="3">
         <v>114.9</v>
       </c>
-      <c r="C29" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D29" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E29" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F29" s="3">
-        <f t="shared" si="3"/>
-        <v>114.9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C29" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D29" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>44239</v>
       </c>
       <c r="B30" s="3">
         <v>115.05</v>
       </c>
-      <c r="C30" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D30" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E30" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F30" s="3">
-        <f t="shared" si="3"/>
-        <v>115.05</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C30" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D30" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>44244</v>
       </c>
       <c r="B31" s="3">
         <v>115.86</v>
       </c>
-      <c r="C31" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D31" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E31" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F31" s="3">
-        <f t="shared" si="3"/>
-        <v>115.86</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C31" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D31" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>44245</v>
       </c>
       <c r="B32" s="3">
         <v>114.61</v>
       </c>
-      <c r="C32" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D32" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E32" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F32" s="3">
-        <f t="shared" si="3"/>
-        <v>114.61</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C32" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D32" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>44246</v>
       </c>
       <c r="B33" s="3">
         <v>113.82</v>
       </c>
-      <c r="C33" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D33" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E33" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F33" s="3">
-        <f t="shared" si="3"/>
-        <v>113.82</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C33" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D33" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>44249</v>
       </c>
       <c r="B34" s="3">
         <v>108.25</v>
       </c>
-      <c r="C34" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D34" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E34" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F34" s="3">
-        <f t="shared" si="3"/>
-        <v>108.25</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C34" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D34" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>44250</v>
       </c>
       <c r="B35" s="3">
         <v>110.76</v>
       </c>
-      <c r="C35" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D35" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E35" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F35" s="3">
-        <f t="shared" si="3"/>
-        <v>110.76</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C35" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D35" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>44251</v>
       </c>
       <c r="B36" s="3">
         <v>111.46</v>
       </c>
-      <c r="C36" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+      <c r="C36" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="D36" s="3">
         <f t="shared" si="1"/>
-        <v>111.46</v>
-      </c>
-      <c r="E36" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F36" s="3">
-        <f t="shared" si="3"/>
-        <v>111.46</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>44252</v>
       </c>
       <c r="B37" s="3">
         <v>107.53</v>
       </c>
-      <c r="C37" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D37" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E37" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F37" s="3" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C37" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D37" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>44253</v>
       </c>
       <c r="B38" s="3">
         <v>105.59</v>
       </c>
-      <c r="C38" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D38" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E38" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F38" s="3" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C38" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D38" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>44256</v>
       </c>
       <c r="B39" s="3">
         <v>105.94</v>
       </c>
-      <c r="C39" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D39" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E39" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F39" s="3" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C39" s="3">
+        <f t="shared" si="0"/>
+        <v>105.94</v>
+      </c>
+      <c r="D39" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>44257</v>
       </c>
       <c r="B40" s="3">
         <v>107.5</v>
       </c>
-      <c r="C40" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D40" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E40" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F40" s="3" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C40" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D40" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>44258</v>
       </c>
       <c r="B41" s="3">
         <v>107.16</v>
       </c>
-      <c r="C41" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D41" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E41" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F41" s="3" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C41" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D41" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>44259</v>
       </c>
       <c r="B42" s="3">
         <v>108.57</v>
       </c>
-      <c r="C42" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D42" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E42" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F42" s="3" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C42" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D42" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>44260</v>
       </c>
       <c r="B43" s="3">
         <v>110.93</v>
       </c>
-      <c r="C43" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D43" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E43" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F43" s="3" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C43" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D43" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>44263</v>
       </c>
       <c r="B44" s="3">
         <v>105.35</v>
       </c>
-      <c r="C44" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D44" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E44" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F44" s="3" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C44" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D44" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44264</v>
       </c>
       <c r="B45" s="3">
         <v>107.19</v>
       </c>
-      <c r="C45" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D45" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E45" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F45" s="3" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C45" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D45" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>44265</v>
       </c>
       <c r="B46" s="3">
         <v>108.63</v>
       </c>
-      <c r="C46" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D46" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E46" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F46" s="3" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C46" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D46" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>44266</v>
       </c>
       <c r="B47" s="3">
         <v>110.45</v>
       </c>
-      <c r="C47" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D47" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E47" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F47" s="3" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C47" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D47" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>44267</v>
       </c>
       <c r="B48" s="3">
         <v>109.68</v>
       </c>
-      <c r="C48" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D48" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E48" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F48" s="3" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C48" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D48" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>44270</v>
       </c>
       <c r="B49" s="3">
         <v>110.66</v>
       </c>
-      <c r="C49" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D49" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E49" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F49" s="3" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C49" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D49" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>44271</v>
       </c>
       <c r="B50" s="3">
         <v>109.69</v>
       </c>
-      <c r="C50" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D50" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E50" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F50" s="3" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C50" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D50" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>44272</v>
       </c>
       <c r="B51" s="3">
         <v>112.05</v>
       </c>
-      <c r="C51" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D51" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E51" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F51" s="3" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C51" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D51" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>44273</v>
       </c>
       <c r="B52" s="3">
         <v>110.5</v>
       </c>
-      <c r="C52" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D52" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E52" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F52" s="3" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C52" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D52" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>44274</v>
       </c>
       <c r="B53" s="3">
         <v>111.7</v>
       </c>
-      <c r="C53" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D53" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E53" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F53" s="3" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C53" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D53" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>44277</v>
       </c>
       <c r="B54" s="3">
         <v>110.69</v>
       </c>
-      <c r="C54" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D54" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E54" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F54" s="3" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C54" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D54" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>44278</v>
       </c>
       <c r="B55" s="3">
         <v>109.02</v>
       </c>
-      <c r="C55" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D55" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E55" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F55" s="3" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C55" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D55" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>44279</v>
       </c>
       <c r="B56" s="3">
         <v>110.33</v>
       </c>
-      <c r="C56" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="D56" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="E56" s="3" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F56" s="3" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
+      <c r="C56" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D56" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="L2">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>$L$2&lt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>$L$2&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$L$2&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">

</xml_diff>

<commit_message>
Gráfico Bolsa de Valores
</commit_message>
<xml_diff>
--- a/7-Gráficos/26. Gráfico de Bolsa de Valores - Material(1).xlsx
+++ b/7-Gráficos/26. Gráfico de Bolsa de Valores - Material(1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\cursos\excel\7-Gráficos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7CEBDE-46AC-481A-8F1C-36C8C37902D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{611CD769-7877-43EE-8A8B-C4219AB1F6C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{25E5CC15-4B2E-4140-8F38-E3ADA3265091}"/>
   </bookViews>
@@ -16,6 +16,19 @@
     <sheet name="Gabarito" sheetId="2" r:id="rId1"/>
     <sheet name="DoZero" sheetId="3" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">DoZero!$A$2:$A$56</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">DoZero!$B$1</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">DoZero!$F$2:$F$56</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">DoZero!$B$2:$B$56</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">DoZero!$C$1</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">DoZero!$C$2:$C$56</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">DoZero!$D$1</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">DoZero!$D$2:$D$56</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">DoZero!$E$1</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">DoZero!$E$2:$E$56</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">DoZero!$F$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -80,7 +93,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,6 +126,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2" tint="-0.749992370372631"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -160,7 +180,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -192,6 +212,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -2537,7 +2560,785 @@
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.4455437635512933E-2"/>
+          <c:y val="3.896103896103896E-2"/>
+          <c:w val="0.90960253337897978"/>
+          <c:h val="0.71150083512288231"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:areaChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>DoZero!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Aux3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="4BFF9C"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>DoZero!$A$2:$A$56</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="55"/>
+                <c:pt idx="0">
+                  <c:v>44200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44201</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44202</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44203</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44204</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44207</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44208</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44209</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44210</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44211</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44214</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44215</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44216</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44217</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44218</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44222</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>44223</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44224</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44225</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>44228</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>44229</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>44230</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>44231</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>44232</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>44235</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>44236</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>44237</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>44238</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>44239</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>44244</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>44245</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>44246</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>44249</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>44250</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>44251</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>44252</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>44253</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>44256</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>44257</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>44258</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44259</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>44260</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>44263</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44264</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44265</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>44266</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>44267</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>44270</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>44271</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>44272</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>44273</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>44274</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>44277</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>44278</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>44279</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>DoZero!$E$2:$E$56</c:f>
+              <c:numCache>
+                <c:formatCode>"R$"\ #,##0.00</c:formatCode>
+                <c:ptCount val="55"/>
+                <c:pt idx="0">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>113.06</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>113.85</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>115.25</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>114.62</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>115.82</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>115.18</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-2A93-42A4-8FAD-1CE0F9F4D8CA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>DoZero!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Aux4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF5B5B"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>DoZero!$A$2:$A$56</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="55"/>
+                <c:pt idx="0">
+                  <c:v>44200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44201</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44202</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44203</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44204</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44207</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44208</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44209</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44210</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44211</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44214</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44215</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44216</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44217</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44218</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44222</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>44223</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44224</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44225</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>44228</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>44229</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>44230</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>44231</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>44232</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>44235</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>44236</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>44237</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>44238</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>44239</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>44244</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>44245</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>44246</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>44249</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>44250</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>44251</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>44252</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>44253</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>44256</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>44257</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>44258</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44259</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>44260</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>44263</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44264</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44265</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>44266</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>44267</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>44270</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>44271</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>44272</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>44273</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>44274</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>44277</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>44278</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>44279</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>DoZero!$F$2:$F$56</c:f>
+              <c:numCache>
+                <c:formatCode>"R$"\ #,##0.00</c:formatCode>
+                <c:ptCount val="55"/>
+                <c:pt idx="0">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-2A93-42A4-8FAD-1CE0F9F4D8CA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1460089935"/>
+        <c:axId val="1460095215"/>
+      </c:areaChart>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -2556,9 +3357,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="9525" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2938,9 +3739,7 @@
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -2949,11 +3748,15 @@
             <c:symbol val="circle"/>
             <c:size val="12"/>
             <c:spPr>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
               <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -3139,169 +3942,169 @@
                 <c:formatCode>"R$"\ #,##0.00</c:formatCode>
                 <c:ptCount val="55"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>113.06</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>105.94</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3329,15 +4132,25 @@
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="12"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:alpha val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -3520,169 +4333,169 @@
                 <c:formatCode>"R$"\ #,##0.00</c:formatCode>
                 <c:ptCount val="55"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>114.55</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>115.18</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3702,6 +4515,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="1460089935"/>
         <c:axId val="1460095215"/>
@@ -3767,9 +4581,8 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -3820,7 +4633,7 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:plotVisOnly val="1"/>
+    <c:plotVisOnly val="0"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
@@ -5353,16 +6166,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>475128</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>8404</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>395007</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>84604</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5437,7 +6250,7 @@
               <a:cs typeface="Calibri"/>
             </a:rPr>
             <a:pPr algn="ctr"/>
-            <a:t>8,13%</a:t>
+            <a:t>1,88%</a:t>
           </a:fld>
           <a:endParaRPr lang="pt-BR" sz="2000" b="1"/>
         </a:p>
@@ -5746,8 +6559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8D9FA79-08E5-4A11-89F3-621F62BC40AC}">
   <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView showGridLines="0" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7170,15 +7983,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6DC53B9-EBCE-429D-8CC4-4E1B53EBCAA8}">
   <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="1" customWidth="1"/>
-    <col min="3" max="6" width="10.5703125" style="1" customWidth="1"/>
+    <col min="3" max="6" width="10.5703125" style="1" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="1"/>
     <col min="8" max="8" width="16.28515625" style="1" customWidth="1"/>
     <col min="9" max="9" width="2.28515625" style="1" customWidth="1"/>
@@ -7224,25 +8037,31 @@
       <c r="B2" s="3">
         <v>114.09</v>
       </c>
-      <c r="C2" s="3">
-        <f>IF($H$2=A2, B2, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="D2" s="3">
-        <f>IF($J$2 = A2, B2, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="H2" s="2">
-        <v>44256</v>
-      </c>
-      <c r="J2" s="2">
-        <v>44202</v>
+      <c r="C2" s="3" t="e">
+        <f>IF($H$2=A2, B2, #N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D2" s="3" t="e">
+        <f>IF($J$2 = A2, B2, #N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E2" s="3" t="e">
+        <f>IF(AND(A2&gt;=$H$2, A2&lt;=$J$2, $L$2 &gt;= 0), B2, #N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F2" s="3" t="e">
+        <f>IF(AND(A2&gt;=$H$2, A2&lt;=$J$2, $L$2 &lt; 0), B2, #N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H2" s="13">
+        <v>44228</v>
+      </c>
+      <c r="J2" s="13">
+        <v>44235</v>
       </c>
       <c r="L2" s="12">
         <f>J3 / H3-1</f>
-        <v>8.1272418350009534E-2</v>
+        <v>1.8751105607641927E-2</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -7252,27 +8071,33 @@
       <c r="B3" s="3">
         <v>114.69</v>
       </c>
-      <c r="C3" s="3">
-        <f t="shared" ref="C3:C56" si="0">IF($H$2=A3, B3, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="D3" s="3">
-        <f t="shared" ref="D3:D56" si="1">IF($J$2 = A3, B3, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="C3" s="3" t="e">
+        <f t="shared" ref="C3:C56" si="0">IF($H$2=A3, B3, #N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D3" s="3" t="e">
+        <f t="shared" ref="D3:D56" si="1">IF($J$2 = A3, B3, #N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E3" s="3" t="e">
+        <f t="shared" ref="E3:E56" si="2">IF(AND(A3&gt;=$H$2, A3&lt;=$J$2, $L$2 &gt;= 0), B3, #N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F3" s="3" t="e">
+        <f t="shared" ref="F3:F56" si="3">IF(AND(A3&gt;=$H$2, A3&lt;=$J$2, $L$2 &lt; 0), B3, #N/A)</f>
+        <v>#N/A</v>
+      </c>
       <c r="H3" s="3">
         <f>VLOOKUP(H2, A:B, 2, 0)</f>
-        <v>105.94</v>
+        <v>113.06</v>
       </c>
       <c r="J3" s="3">
         <f>VLOOKUP(J2, A:B, 2, 0)</f>
-        <v>114.55</v>
+        <v>115.18</v>
       </c>
       <c r="L3" s="3">
         <f>J3 - H3</f>
-        <v>8.61</v>
+        <v>2.1200000000000045</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -7282,16 +8107,22 @@
       <c r="B4" s="3">
         <v>114.55</v>
       </c>
-      <c r="C4" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D4" s="3">
-        <f t="shared" si="1"/>
-        <v>114.55</v>
-      </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="C4" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D4" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E4" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F4" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -7300,16 +8131,22 @@
       <c r="B5" s="3">
         <v>118.37</v>
       </c>
-      <c r="C5" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D5" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="C5" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D5" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E5" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F5" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -7318,16 +8155,22 @@
       <c r="B6" s="3">
         <v>120.4</v>
       </c>
-      <c r="C6" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D6" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+      <c r="C6" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D6" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E6" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F6" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
@@ -7336,16 +8179,22 @@
       <c r="B7" s="3">
         <v>118.62</v>
       </c>
-      <c r="C7" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D7" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="C7" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D7" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E7" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F7" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -7354,16 +8203,22 @@
       <c r="B8" s="3">
         <v>119.45</v>
       </c>
-      <c r="C8" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D8" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
+      <c r="C8" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D8" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E8" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F8" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
@@ -7372,16 +8227,22 @@
       <c r="B9" s="3">
         <v>117.36</v>
       </c>
-      <c r="C9" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D9" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
+      <c r="C9" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D9" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E9" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F9" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -7390,16 +8251,22 @@
       <c r="B10" s="3">
         <v>118.68</v>
       </c>
-      <c r="C10" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D10" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
+      <c r="C10" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D10" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E10" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F10" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
@@ -7408,16 +8275,22 @@
       <c r="B11" s="3">
         <v>115.78</v>
       </c>
-      <c r="C11" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D11" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
+      <c r="C11" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D11" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E11" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F11" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
@@ -7426,16 +8299,22 @@
       <c r="B12" s="3">
         <v>116.54</v>
       </c>
-      <c r="C12" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D12" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
+      <c r="C12" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D12" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E12" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F12" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
@@ -7444,16 +8323,22 @@
       <c r="B13" s="3">
         <v>116</v>
       </c>
-      <c r="C13" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D13" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
+      <c r="C13" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D13" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E13" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F13" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -7462,16 +8347,22 @@
       <c r="B14" s="3">
         <v>115.24</v>
       </c>
-      <c r="C14" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D14" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
+      <c r="C14" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D14" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E14" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F14" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
@@ -7480,16 +8371,22 @@
       <c r="B15" s="3">
         <v>113.81</v>
       </c>
-      <c r="C15" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D15" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
+      <c r="C15" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D15" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E15" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F15" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
@@ -7498,16 +8395,22 @@
       <c r="B16" s="3">
         <v>113.18</v>
       </c>
-      <c r="C16" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D16" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
+      <c r="C16" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D16" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E16" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F16" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
@@ -7516,16 +8419,22 @@
       <c r="B17" s="3">
         <v>112.08</v>
       </c>
-      <c r="C17" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D17" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
+      <c r="C17" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D17" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E17" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F17" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
@@ -7534,16 +8443,22 @@
       <c r="B18" s="3">
         <v>110.96</v>
       </c>
-      <c r="C18" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D18" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
+      <c r="C18" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D18" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E18" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F18" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
@@ -7552,16 +8467,22 @@
       <c r="B19" s="3">
         <v>114.51</v>
       </c>
-      <c r="C19" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D19" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
+      <c r="C19" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D19" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E19" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F19" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
@@ -7570,16 +8491,22 @@
       <c r="B20" s="3">
         <v>110.56</v>
       </c>
-      <c r="C20" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D20" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
+      <c r="C20" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D20" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E20" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F20" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
@@ -7590,14 +8517,20 @@
       </c>
       <c r="C21" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D21" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
+        <v>113.06</v>
+      </c>
+      <c r="D21" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" si="2"/>
+        <v>113.06</v>
+      </c>
+      <c r="F21" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
@@ -7606,16 +8539,22 @@
       <c r="B22" s="3">
         <v>113.85</v>
       </c>
-      <c r="C22" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D22" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
+      <c r="C22" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D22" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E22" s="3">
+        <f t="shared" si="2"/>
+        <v>113.85</v>
+      </c>
+      <c r="F22" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
@@ -7624,16 +8563,22 @@
       <c r="B23" s="3">
         <v>115.25</v>
       </c>
-      <c r="C23" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D23" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
+      <c r="C23" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D23" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" si="2"/>
+        <v>115.25</v>
+      </c>
+      <c r="F23" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
@@ -7642,16 +8587,22 @@
       <c r="B24" s="3">
         <v>114.62</v>
       </c>
-      <c r="C24" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D24" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
+      <c r="C24" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D24" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" si="2"/>
+        <v>114.62</v>
+      </c>
+      <c r="F24" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
@@ -7660,16 +8611,22 @@
       <c r="B25" s="3">
         <v>115.82</v>
       </c>
-      <c r="C25" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D25" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
+      <c r="C25" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D25" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E25" s="3">
+        <f t="shared" si="2"/>
+        <v>115.82</v>
+      </c>
+      <c r="F25" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
@@ -7678,16 +8635,22 @@
       <c r="B26" s="3">
         <v>115.18</v>
       </c>
-      <c r="C26" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="C26" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
       </c>
       <c r="D26" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
+        <v>115.18</v>
+      </c>
+      <c r="E26" s="3">
+        <f t="shared" si="2"/>
+        <v>115.18</v>
+      </c>
+      <c r="F26" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
@@ -7696,16 +8659,22 @@
       <c r="B27" s="3">
         <v>114.91</v>
       </c>
-      <c r="C27" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D27" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
+      <c r="C27" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D27" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E27" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F27" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
@@ -7714,16 +8683,22 @@
       <c r="B28" s="3">
         <v>113.92</v>
       </c>
-      <c r="C28" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D28" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
+      <c r="C28" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D28" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E28" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F28" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
@@ -7732,16 +8707,22 @@
       <c r="B29" s="3">
         <v>114.9</v>
       </c>
-      <c r="C29" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D29" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
+      <c r="C29" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D29" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E29" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F29" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
@@ -7750,16 +8731,22 @@
       <c r="B30" s="3">
         <v>115.05</v>
       </c>
-      <c r="C30" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D30" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
+      <c r="C30" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D30" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E30" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F30" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
@@ -7768,16 +8755,22 @@
       <c r="B31" s="3">
         <v>115.86</v>
       </c>
-      <c r="C31" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D31" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
+      <c r="C31" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D31" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E31" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F31" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
@@ -7786,16 +8779,22 @@
       <c r="B32" s="3">
         <v>114.61</v>
       </c>
-      <c r="C32" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D32" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
+      <c r="C32" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D32" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E32" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F32" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
@@ -7804,16 +8803,22 @@
       <c r="B33" s="3">
         <v>113.82</v>
       </c>
-      <c r="C33" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D33" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
+      <c r="C33" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D33" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E33" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F33" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
@@ -7822,16 +8827,22 @@
       <c r="B34" s="3">
         <v>108.25</v>
       </c>
-      <c r="C34" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D34" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
+      <c r="C34" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D34" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E34" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F34" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
@@ -7840,16 +8851,22 @@
       <c r="B35" s="3">
         <v>110.76</v>
       </c>
-      <c r="C35" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D35" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
+      <c r="C35" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D35" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E35" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F35" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
@@ -7858,16 +8875,22 @@
       <c r="B36" s="3">
         <v>111.46</v>
       </c>
-      <c r="C36" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D36" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
+      <c r="C36" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D36" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E36" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F36" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
@@ -7876,16 +8899,22 @@
       <c r="B37" s="3">
         <v>107.53</v>
       </c>
-      <c r="C37" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D37" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
+      <c r="C37" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D37" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E37" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F37" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
@@ -7894,16 +8923,22 @@
       <c r="B38" s="3">
         <v>105.59</v>
       </c>
-      <c r="C38" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D38" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
+      <c r="C38" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D38" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E38" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F38" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
@@ -7912,16 +8947,22 @@
       <c r="B39" s="3">
         <v>105.94</v>
       </c>
-      <c r="C39" s="3">
-        <f t="shared" si="0"/>
-        <v>105.94</v>
-      </c>
-      <c r="D39" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
+      <c r="C39" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D39" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E39" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F39" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
@@ -7930,16 +8971,22 @@
       <c r="B40" s="3">
         <v>107.5</v>
       </c>
-      <c r="C40" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D40" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
+      <c r="C40" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D40" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E40" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F40" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
@@ -7948,16 +8995,22 @@
       <c r="B41" s="3">
         <v>107.16</v>
       </c>
-      <c r="C41" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D41" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
+      <c r="C41" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D41" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E41" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F41" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
@@ -7966,16 +9019,22 @@
       <c r="B42" s="3">
         <v>108.57</v>
       </c>
-      <c r="C42" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D42" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
+      <c r="C42" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D42" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E42" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F42" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
@@ -7984,16 +9043,22 @@
       <c r="B43" s="3">
         <v>110.93</v>
       </c>
-      <c r="C43" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D43" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
+      <c r="C43" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D43" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E43" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F43" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
@@ -8002,16 +9067,22 @@
       <c r="B44" s="3">
         <v>105.35</v>
       </c>
-      <c r="C44" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D44" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
+      <c r="C44" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D44" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E44" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F44" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
@@ -8020,16 +9091,22 @@
       <c r="B45" s="3">
         <v>107.19</v>
       </c>
-      <c r="C45" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D45" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
+      <c r="C45" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D45" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E45" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F45" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
@@ -8038,16 +9115,22 @@
       <c r="B46" s="3">
         <v>108.63</v>
       </c>
-      <c r="C46" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D46" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
+      <c r="C46" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D46" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E46" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F46" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
@@ -8056,16 +9139,22 @@
       <c r="B47" s="3">
         <v>110.45</v>
       </c>
-      <c r="C47" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D47" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
+      <c r="C47" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D47" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E47" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F47" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
@@ -8074,16 +9163,22 @@
       <c r="B48" s="3">
         <v>109.68</v>
       </c>
-      <c r="C48" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D48" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
+      <c r="C48" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D48" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E48" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F48" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
@@ -8092,16 +9187,22 @@
       <c r="B49" s="3">
         <v>110.66</v>
       </c>
-      <c r="C49" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D49" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
+      <c r="C49" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D49" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E49" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F49" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
@@ -8110,16 +9211,22 @@
       <c r="B50" s="3">
         <v>109.69</v>
       </c>
-      <c r="C50" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D50" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
+      <c r="C50" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D50" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E50" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F50" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
@@ -8128,16 +9235,22 @@
       <c r="B51" s="3">
         <v>112.05</v>
       </c>
-      <c r="C51" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D51" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
+      <c r="C51" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D51" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E51" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F51" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
@@ -8146,16 +9259,22 @@
       <c r="B52" s="3">
         <v>110.5</v>
       </c>
-      <c r="C52" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D52" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
+      <c r="C52" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D52" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E52" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F52" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
@@ -8164,16 +9283,22 @@
       <c r="B53" s="3">
         <v>111.7</v>
       </c>
-      <c r="C53" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D53" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
+      <c r="C53" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D53" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E53" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F53" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
@@ -8182,16 +9307,22 @@
       <c r="B54" s="3">
         <v>110.69</v>
       </c>
-      <c r="C54" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D54" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
+      <c r="C54" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D54" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E54" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F54" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
@@ -8200,16 +9331,22 @@
       <c r="B55" s="3">
         <v>109.02</v>
       </c>
-      <c r="C55" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D55" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
+      <c r="C55" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D55" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E55" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F55" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
@@ -8218,16 +9355,22 @@
       <c r="B56" s="3">
         <v>110.33</v>
       </c>
-      <c r="C56" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D56" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
+      <c r="C56" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D56" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E56" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F56" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="L2">

</xml_diff>